<commit_message>
fixing layout perubahan kolom table
</commit_message>
<xml_diff>
--- a/public/template/Template_Urjab.xlsx
+++ b/public/template/Template_Urjab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\DIRJAB-IP\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8AA596-4CBD-4DB4-B241-834860173AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7E562E-BB48-4DE6-A675-9E8BFB1118FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -422,75 +422,69 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -881,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -922,56 +916,56 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="39"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -984,15 +978,15 @@
     </row>
     <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
@@ -1002,10 +996,10 @@
       <c r="D11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
@@ -1015,10 +1009,10 @@
       <c r="D12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
@@ -1028,10 +1022,10 @@
       <c r="D13" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
@@ -1041,10 +1035,10 @@
       <c r="D14" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
@@ -1054,10 +1048,10 @@
       <c r="D15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
@@ -1067,10 +1061,10 @@
       <c r="D16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -1082,24 +1076,24 @@
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
     </row>
     <row r="20" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="48"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
@@ -1121,45 +1115,45 @@
     </row>
     <row r="23" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30" t="s">
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="30"/>
+      <c r="H24" s="35"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="22">
         <v>1</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="47" t="s">
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="27"/>
+      <c r="H25" s="36"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E26"/>
@@ -1242,30 +1236,30 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="C53" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30" t="s">
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="H53" s="30"/>
+      <c r="H53" s="35"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="16"/>
@@ -1301,13 +1295,13 @@
       <c r="E62"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
       <c r="E63"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
+      <c r="B64" s="42"/>
+      <c r="C64" s="42"/>
       <c r="E64"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
@@ -1317,33 +1311,33 @@
       <c r="E66"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="25"/>
-      <c r="C67" s="26"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="44"/>
       <c r="E67"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="25"/>
-      <c r="C68" s="26"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="44"/>
       <c r="E68"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="25"/>
-      <c r="C69" s="26"/>
+      <c r="B69" s="43"/>
+      <c r="C69" s="44"/>
       <c r="E69"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="25"/>
-      <c r="C70" s="26"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="44"/>
       <c r="E70"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="25"/>
-      <c r="C71" s="26"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="44"/>
       <c r="E71"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="25"/>
-      <c r="C72" s="26"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="44"/>
       <c r="E72"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
@@ -1353,23 +1347,23 @@
       <c r="E74"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="25"/>
-      <c r="C75" s="26"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="44"/>
       <c r="E75"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="25"/>
-      <c r="C76" s="26"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="44"/>
       <c r="E76"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="25"/>
-      <c r="C77" s="26"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="44"/>
       <c r="E77"/>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="25"/>
-      <c r="C78" s="26"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="44"/>
       <c r="E78"/>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
@@ -1879,25 +1873,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="35">
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="A4:E5"/>
-    <mergeCell ref="A6:E7"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="G24:H24"/>
     <mergeCell ref="B69:C69"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="G25:H25"/>
@@ -1914,6 +1889,25 @@
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="A4:E5"/>
+    <mergeCell ref="A6:E7"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>